<commit_message>
More boulders, About page
</commit_message>
<xml_diff>
--- a/data/Hueco/Ticklist.xlsx
+++ b/data/Hueco/Ticklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
   <si>
     <t>Areas</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>Zax Rock</t>
+  </si>
+  <si>
+    <t>The Kitchen</t>
+  </si>
+  <si>
+    <t>Power of Silence</t>
+  </si>
+  <si>
+    <t>Gums Boulder</t>
+  </si>
+  <si>
+    <t>Look Sharp Rock</t>
+  </si>
+  <si>
+    <t>Sign of the cross wall</t>
+  </si>
+  <si>
+    <t>Term Boulder</t>
   </si>
 </sst>
 </file>
@@ -987,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,169 +1122,205 @@
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Boulders, places, boulder labels
</commit_message>
<xml_diff>
--- a/data/Hueco/Ticklist.xlsx
+++ b/data/Hueco/Ticklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
   <si>
     <t>Areas</t>
   </si>
@@ -361,13 +361,190 @@
   </si>
   <si>
     <t>Term Boulder</t>
+  </si>
+  <si>
+    <t>Diaphanous Boulder</t>
+  </si>
+  <si>
+    <t>Choss Wall</t>
+  </si>
+  <si>
+    <t>Micheal Kenyon</t>
+  </si>
+  <si>
+    <t>Donkey Head Rock</t>
+  </si>
+  <si>
+    <t>Hawkbill Rock</t>
+  </si>
+  <si>
+    <t>Outhouse Rock</t>
+  </si>
+  <si>
+    <t>Warm Up Boulder</t>
+  </si>
+  <si>
+    <t>Warm Up Wall</t>
+  </si>
+  <si>
+    <t>Mammary Lane</t>
+  </si>
+  <si>
+    <t>V-Obsession</t>
+  </si>
+  <si>
+    <t>Theater of the Absurd</t>
+  </si>
+  <si>
+    <t>Asylum Crack</t>
+  </si>
+  <si>
+    <t>Mopboys Roof</t>
+  </si>
+  <si>
+    <t>Bleeding Brothers Roof</t>
+  </si>
+  <si>
+    <t>Brownstone Rock</t>
+  </si>
+  <si>
+    <t>Lunch Rocks</t>
+  </si>
+  <si>
+    <t>Scarface Rock</t>
+  </si>
+  <si>
+    <t>Turtle Wax</t>
+  </si>
+  <si>
+    <t>Smooth Moves</t>
+  </si>
+  <si>
+    <t>Present Arms</t>
+  </si>
+  <si>
+    <t>Malice Boulder</t>
+  </si>
+  <si>
+    <t>The Pyramid</t>
+  </si>
+  <si>
+    <t>The There Stack</t>
+  </si>
+  <si>
+    <t>Hairy Boulder</t>
+  </si>
+  <si>
+    <t>Scary Boulder</t>
+  </si>
+  <si>
+    <t>Not Quite So Scary Boulder</t>
+  </si>
+  <si>
+    <t>The Coprolith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dab </t>
+  </si>
+  <si>
+    <t>Slab of the Poseurs</t>
+  </si>
+  <si>
+    <t>The Scruple</t>
+  </si>
+  <si>
+    <t>North Deliverance</t>
+  </si>
+  <si>
+    <t>South Deliverance</t>
+  </si>
+  <si>
+    <t>Holy Cow Boulder</t>
+  </si>
+  <si>
+    <t>End Loop Boulder</t>
+  </si>
+  <si>
+    <t>Fencehopper Rock</t>
+  </si>
+  <si>
+    <t>Icarus Boulder</t>
+  </si>
+  <si>
+    <t>Wall of Early Morning Fright</t>
+  </si>
+  <si>
+    <t>End of the Cave</t>
+  </si>
+  <si>
+    <t>The South-Facing Wall</t>
+  </si>
+  <si>
+    <t>The North-Facing Wall</t>
+  </si>
+  <si>
+    <t>The Russet</t>
+  </si>
+  <si>
+    <t>The Baker</t>
+  </si>
+  <si>
+    <t>Baby Baker</t>
+  </si>
+  <si>
+    <t>Rotten Potato</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Shake Rock</t>
+  </si>
+  <si>
+    <t>Little Big Time</t>
+  </si>
+  <si>
+    <t>Fern Wall</t>
+  </si>
+  <si>
+    <t>Main Wall</t>
+  </si>
+  <si>
+    <t>The Grenade</t>
+  </si>
+  <si>
+    <t>Babyface Boulder</t>
+  </si>
+  <si>
+    <t>Aftershave Rock</t>
+  </si>
+  <si>
+    <t>Reject Rock</t>
+  </si>
+  <si>
+    <t>Army of Darkness</t>
+  </si>
+  <si>
+    <t>Attitude Problem</t>
+  </si>
+  <si>
+    <t>Couch Potato</t>
+  </si>
+  <si>
+    <t>South Groupie Alert Boulder</t>
+  </si>
+  <si>
+    <t>North Groupie Alert Boulder</t>
+  </si>
+  <si>
+    <t>See-Thru Boulder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,8 +567,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +620,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -444,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -453,6 +657,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,42 +1244,42 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1079,21 +1288,21 @@
       <c r="B8" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1102,14 +1311,14 @@
       <c r="B11" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1125,28 +1334,28 @@
       <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1155,174 +1364,584 @@
       <c r="B18" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="B54" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+      <c r="B56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="9"/>
+      <c r="B57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="B59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="B65" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="B67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="9"/>
+      <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="9"/>
+      <c r="B69" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="B72" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" t="s">
+        <v>157</v>
+      </c>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="9"/>
+      <c r="B75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="B77" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="B78" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="9"/>
+      <c r="B79" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="9"/>
+      <c r="B80" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="9"/>
+      <c r="B81" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="9"/>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="B83" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="9"/>
+      <c r="B86" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B87" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="B88" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+      <c r="B89" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="9"/>
+      <c r="B90" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="B91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="9"/>
+      <c r="B92" t="s">
+        <v>168</v>
+      </c>
+      <c r="C92" s="6"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="B93" t="s">
+        <v>171</v>
+      </c>
+      <c r="C93" s="6"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="6"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>173</v>
+      </c>
+      <c r="C95" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>